<commit_message>
test ragas fait avec 5 données
</commit_message>
<xml_diff>
--- a/data/output/resultats_ragas_evaluation.xlsx
+++ b/data/output/resultats_ragas_evaluation.xlsx
@@ -501,13 +501,17 @@
           <t>Eldershade</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.625</v>
+      </c>
       <c r="F2" t="n">
-        <v>0.6356910495188841</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
+        <v>0.6959323534415676</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.9999999999</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -534,15 +538,21 @@
           <t>A young shepherd named Elian.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.4858680360343469</v>
+      </c>
       <c r="F3" t="n">
         <v>0.5038801405355749</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
       <c r="H3" t="n">
         <v>0.9999999999</v>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -565,15 +575,21 @@
           <t>Animals became unusually calm and would follow humans peacefully.</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.5186869123087048</v>
+      </c>
       <c r="F4" t="n">
         <v>0.6436697640865007</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0.75</v>
+      </c>
       <c r="H4" t="n">
         <v>0.9999999999</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -596,11 +612,15 @@
           <t>The villagers gathered around the stone for warmth and it emitted a gentle heat that kept them safe when fires failed.</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.5582612362888708</v>
+      </c>
       <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
+        <v>0.7966863272106656</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
       <c r="H5" t="n">
         <v>0.9999999999</v>
       </c>
@@ -626,18 +646,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mira the Wise.</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>Only the village elder, Mira the Wise, was permitted to touch the stone with her bare hands.</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4523436136211799</v>
+      </c>
       <c r="F6" t="n">
-        <v>0.4871973919868788</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
       <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
+        <v>0.9999999999</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Réorganisation du code en différents dossier et sous dossier pour plus de visibilité
</commit_message>
<xml_diff>
--- a/data/output/resultats_ragas_evaluation.xlsx
+++ b/data/output/resultats_ragas_evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,7 +505,7 @@
         <v>0.625</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6959323534415676</v>
+        <v>0.5200242194585092</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.4858680360343469</v>
+        <v>0.5608680360343469</v>
       </c>
       <c r="F3" t="n">
         <v>0.5038801405355749</v>
@@ -551,117 +551,6 @@
         <v>0.9999999999</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>What unusual effect did the stone have on animals?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Animals that came close to the glowing stone became unusually calm and would follow humans peacefully. Even wolves and wild boars showed no aggression near the stone.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>They became calm and peaceful, even wild animals like wolves.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Animals became unusually calm and would follow humans peacefully.</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.5186869123087048</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.6436697640865007</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.9999999999</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>How did the villagers use the stone during the winter?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>During the harsh winters, the villagers gathered around the stone for warmth. It emitted a gentle heat that kept them safe when fires failed.</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>They used it for warmth when fires failed during winter.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>The villagers gathered around the stone for warmth and it emitted a gentle heat that kept them safe when fires failed.</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0.5582612362888708</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.7966863272106656</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.9999999999</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Who was the only person allowed to touch the stone directly?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Only the village elder, known as Mira the Wise, was permitted to touch the stone with her bare hands. Others had to use thick gloves or wooden tools.</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Mira the Wise</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Only the village elder, Mira the Wise, was permitted to touch the stone with her bare hands.</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.4523436136211799</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.9999999999</v>
-      </c>
-      <c r="I6" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>